<commit_message>
end of week 5 day 1 code updated
</commit_message>
<xml_diff>
--- a/planet.xlsx
+++ b/planet.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,21 @@
           <t>Feature</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Discoverer</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Year of Discovery</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Composition</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -486,7 +501,22 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Mercury has the most eccentric orbit of all the planets.</t>
+          <t>Eccentric orbit</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Iron</t>
         </is>
       </c>
     </row>
@@ -516,7 +546,22 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Venus has a runaway greenhouse effect that makes it hotter than Mercury</t>
+          <t>runaway greenhouse</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Carbon dioxide</t>
         </is>
       </c>
     </row>
@@ -546,7 +591,22 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Earth is the only planet known to support life and has liquid water on its surface.</t>
+          <t>only planet known to support life</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Nitrogen and oxygen</t>
         </is>
       </c>
     </row>
@@ -576,7 +636,22 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Mars has the largest volcano in the solar system.</t>
+          <t>largest volcano</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Iron oxide</t>
         </is>
       </c>
     </row>
@@ -606,7 +681,22 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Jupiter's Great Red Spot is a massive storm that's been raging for at least 400 years.</t>
+          <t>Red Spot is a massive storm</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Mostly hydrogen and helium</t>
         </is>
       </c>
     </row>
@@ -636,7 +726,22 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Saturn's rings are the most extensive and brightest in the solar system.</t>
+          <t>Saturn's rings are the most extensive</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Mostly hydrogen and helium</t>
         </is>
       </c>
     </row>
@@ -666,7 +771,22 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Uranus rotates on its side, making it unique among the planets.</t>
+          <t>Uranus rotates on its side</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Sir William Herschel</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>1781</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Hydrogen, helium, and methane</t>
         </is>
       </c>
     </row>
@@ -696,7 +816,67 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Neptune has the strongest winds in the solar system.</t>
+          <t>Neptune has the strongest winds</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Johann Galle and Urbain Le Verrier</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>1846</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Hydrogen, helium, and methane</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Pluto</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>-229°C</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>1,188.3 km</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Brownish-yellow</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>two-thirds the width of Earth's moon</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Clyde Tombaugh</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>1930</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Mostly ice and rock</t>
         </is>
       </c>
     </row>

</xml_diff>